<commit_message>
Scenario 1 ready (no parameter)
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/output/output_modelo MM - TALCA 28.12_v6 - E1.xlsx
+++ b/Code/Limpio/Excels/output/output_modelo MM - TALCA 28.12_v6 - E1.xlsx
@@ -10,13 +10,14 @@
     <sheet name="BBDD - Error Actual" sheetId="1" r:id="rId1"/>
     <sheet name="Resultados loc" sheetId="2" r:id="rId2"/>
     <sheet name="Inicial y final" sheetId="3" r:id="rId3"/>
+    <sheet name="RESUMEN E1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="223">
   <si>
     <t>LOCALIDAD</t>
   </si>
@@ -655,6 +656,36 @@
   </si>
   <si>
     <t>V_sub f</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Scenario 1: medidores con VAN &gt; 0</t>
+  </si>
+  <si>
+    <t>Consumo (m3/año)</t>
+  </si>
+  <si>
+    <t>Submedición Con Proyecto (m3/año)</t>
+  </si>
+  <si>
+    <t>Submedición Sin Proyecto (m3)</t>
+  </si>
+  <si>
+    <t>Diferencial (volumen recuperado, m3/año)</t>
+  </si>
+  <si>
+    <t>Diferencial (% c/r consumo renovados)</t>
+  </si>
+  <si>
+    <t>Ingresos volumen recuperado ($/año)</t>
+  </si>
+  <si>
+    <t>Con Proyecto - Error ponderado final</t>
+  </si>
+  <si>
+    <t>Sin Proyecto - Error ponderado final</t>
   </si>
 </sst>
 </file>
@@ -2900,34 +2931,34 @@
         <v>-1887.274750418313</v>
       </c>
       <c r="DF5">
-        <v>-808772.7904866072</v>
+        <v>-821169.4864866072</v>
       </c>
       <c r="DG5">
-        <v>-242631.8371459822</v>
+        <v>-246350.8459459821</v>
       </c>
       <c r="DH5">
-        <v>-242631.8371459822</v>
+        <v>-246350.8459459821</v>
       </c>
       <c r="DI5">
-        <v>-242631.8371459822</v>
+        <v>-246350.8459459821</v>
       </c>
       <c r="DJ5">
-        <v>-80877.27904866077</v>
+        <v>-82116.94864866079</v>
       </c>
       <c r="DK5">
-        <v>727895.5114379465</v>
+        <v>739052.5378379466</v>
       </c>
       <c r="DL5">
-        <v>-219397.2602201853</v>
+        <v>-223116.2690201853</v>
       </c>
       <c r="DM5">
-        <v>-213802.3512701397</v>
+        <v>-217521.3600701397</v>
       </c>
       <c r="DN5">
-        <v>-210123.8034333892</v>
+        <v>-213842.8122333892</v>
       </c>
       <c r="DO5">
-        <v>-45619.41482443192</v>
+        <v>-46859.08442443195</v>
       </c>
       <c r="DP5">
         <v>37454.63935763667</v>
@@ -2963,49 +2994,49 @@
         <v>48440.05192740329</v>
       </c>
       <c r="EA5">
-        <v>-219397.2602201853</v>
+        <v>-223116.2690201853</v>
       </c>
       <c r="EB5">
-        <v>-433199.611490325</v>
+        <v>-440637.629090325</v>
       </c>
       <c r="EC5">
-        <v>-643323.4149237141</v>
+        <v>-654480.4413237141</v>
       </c>
       <c r="ED5">
-        <v>-688942.829748146</v>
+        <v>-701339.525748146</v>
       </c>
       <c r="EE5">
-        <v>-651488.1903905093</v>
+        <v>-663884.8863905093</v>
       </c>
       <c r="EF5">
-        <v>-612199.573608216</v>
+        <v>-624596.269608216</v>
       </c>
       <c r="EG5">
-        <v>-571344.1527692167</v>
+        <v>-583740.8487692167</v>
       </c>
       <c r="EH5">
-        <v>-529118.0229122281</v>
+        <v>-541514.7189122281</v>
       </c>
       <c r="EI5">
-        <v>-485673.6092207374</v>
+        <v>-498070.3052207374</v>
       </c>
       <c r="EJ5">
-        <v>-441129.9458923203</v>
+        <v>-453526.6418923203</v>
       </c>
       <c r="EK5">
-        <v>-395589.8436566967</v>
+        <v>-407986.5396566967</v>
       </c>
       <c r="EL5">
-        <v>-349136.3352019755</v>
+        <v>-361533.0312019755</v>
       </c>
       <c r="EM5">
-        <v>-301839.673219674</v>
+        <v>-314236.369219674</v>
       </c>
       <c r="EN5">
-        <v>-253758.001202705</v>
+        <v>-266154.697202705</v>
       </c>
       <c r="EO5">
-        <v>-205317.9492753017</v>
+        <v>-217714.6452753017</v>
       </c>
       <c r="EP5">
         <v>0</v>
@@ -3098,7 +3129,7 @@
         <v>48440.05192740329</v>
       </c>
       <c r="FT5">
-        <v>73639.8641730104</v>
+        <v>69440.67433944368</v>
       </c>
     </row>
     <row r="6" spans="1:176">
@@ -3430,34 +3461,34 @@
         <v>-2496.394433237535</v>
       </c>
       <c r="DF6">
-        <v>-160396.8907078734</v>
+        <v>-172793.5867078734</v>
       </c>
       <c r="DG6">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DH6">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DI6">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DJ6">
-        <v>-16039.68907078734</v>
+        <v>-17279.35867078736</v>
       </c>
       <c r="DK6">
-        <v>144357.2016370861</v>
+        <v>155514.2280370861</v>
       </c>
       <c r="DL6">
-        <v>1024.059460959637</v>
+        <v>-2694.949339040359</v>
       </c>
       <c r="DM6">
-        <v>3517.62562559326</v>
+        <v>-201.3831744067356</v>
       </c>
       <c r="DN6">
-        <v>5649.18839601551</v>
+        <v>1930.179596015514</v>
       </c>
       <c r="DO6">
-        <v>39594.17449018311</v>
+        <v>38354.50489018309</v>
       </c>
       <c r="DP6">
         <v>57292.58132540926</v>
@@ -3493,16 +3524,16 @@
         <v>64074.12378642998</v>
       </c>
       <c r="EA6">
-        <v>1024.059460959637</v>
+        <v>-2694.949339040359</v>
       </c>
       <c r="EB6">
-        <v>3517.62562559326</v>
+        <v>-2896.332513447094</v>
       </c>
       <c r="EC6">
-        <v>5649.18839601551</v>
+        <v>-966.1529174315801</v>
       </c>
       <c r="ED6">
-        <v>39594.17449018311</v>
+        <v>37388.35197275151</v>
       </c>
       <c r="EE6">
         <v>57292.58132540926</v>
@@ -3538,16 +3569,16 @@
         <v>64074.12378642998</v>
       </c>
       <c r="EP6">
-        <v>-276.4960544591021</v>
+        <v>0</v>
       </c>
       <c r="EQ6">
-        <v>-949.7589189101803</v>
+        <v>0</v>
       </c>
       <c r="ER6">
-        <v>-1525.280866924188</v>
+        <v>0</v>
       </c>
       <c r="ES6">
-        <v>-10690.42711234944</v>
+        <v>-10094.85503264291</v>
       </c>
       <c r="ET6">
         <v>-15468.9969578605</v>
@@ -3583,16 +3614,16 @@
         <v>-17300.0134223361</v>
       </c>
       <c r="FE6">
-        <v>48866.63061886257</v>
+        <v>49143.12667332167</v>
       </c>
       <c r="FF6">
-        <v>50686.93391904511</v>
+        <v>51636.69283795529</v>
       </c>
       <c r="FG6">
-        <v>52242.97474145336</v>
+        <v>53768.25560837754</v>
       </c>
       <c r="FH6">
-        <v>44943.43644862101</v>
+        <v>45539.00852832754</v>
       </c>
       <c r="FI6">
         <v>41823.58436754876</v>
@@ -3628,7 +3659,7 @@
         <v>46774.11036409388</v>
       </c>
       <c r="FT6">
-        <v>370317.0486244283</v>
+        <v>368905.2651620624</v>
       </c>
     </row>
     <row r="7" spans="1:176">
@@ -3960,34 +3991,34 @@
         <v>-1140.049279035991</v>
       </c>
       <c r="DF7">
-        <v>-160396.8907078734</v>
+        <v>-172793.5867078734</v>
       </c>
       <c r="DG7">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DH7">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DI7">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DJ7">
-        <v>-16039.68907078734</v>
+        <v>-17279.35867078736</v>
       </c>
       <c r="DK7">
-        <v>144357.2016370861</v>
+        <v>155514.2280370861</v>
       </c>
       <c r="DL7">
-        <v>-26503.68845944729</v>
+        <v>-30222.69725944728</v>
       </c>
       <c r="DM7">
-        <v>-25231.37289411987</v>
+        <v>-28950.38169411987</v>
       </c>
       <c r="DN7">
-        <v>-24161.66505196587</v>
+        <v>-27880.67385196586</v>
       </c>
       <c r="DO7">
-        <v>8842.578377746493</v>
+        <v>7602.90877774647</v>
       </c>
       <c r="DP7">
         <v>25696.87767473527</v>
@@ -4023,28 +4054,28 @@
         <v>29261.26482859049</v>
       </c>
       <c r="EA7">
-        <v>-26503.68845944729</v>
+        <v>-30222.69725944728</v>
       </c>
       <c r="EB7">
-        <v>-51735.06135356716</v>
+        <v>-59173.07895356715</v>
       </c>
       <c r="EC7">
-        <v>-75896.72640553303</v>
+        <v>-87053.752805533</v>
       </c>
       <c r="ED7">
-        <v>-67054.14802778653</v>
+        <v>-79450.84402778653</v>
       </c>
       <c r="EE7">
-        <v>-41357.27035305127</v>
+        <v>-53753.96635305126</v>
       </c>
       <c r="EF7">
-        <v>-14930.63642092184</v>
+        <v>-27327.33242092184</v>
       </c>
       <c r="EG7">
-        <v>12153.65289265484</v>
+        <v>-243.0431073451546</v>
       </c>
       <c r="EH7">
-        <v>27684.24052656692</v>
+        <v>27441.19741922177</v>
       </c>
       <c r="EI7">
         <v>28235.80197424061</v>
@@ -4086,10 +4117,10 @@
         <v>0</v>
       </c>
       <c r="EV7">
-        <v>-3281.486281016807</v>
+        <v>0</v>
       </c>
       <c r="EW7">
-        <v>-7474.74494217307</v>
+        <v>-7409.123303189877</v>
       </c>
       <c r="EX7">
         <v>-7623.666533044965</v>
@@ -4131,10 +4162,10 @@
         <v>26426.63393212942</v>
       </c>
       <c r="FK7">
-        <v>23802.80303255988</v>
+        <v>27084.28931357669</v>
       </c>
       <c r="FL7">
-        <v>20209.49558439385</v>
+        <v>20275.11722337704</v>
       </c>
       <c r="FM7">
         <v>20612.13544119565</v>
@@ -4158,7 +4189,7 @@
         <v>21360.72332487106</v>
       </c>
       <c r="FT7">
-        <v>153304.3315881218</v>
+        <v>151186.8788804009</v>
       </c>
     </row>
     <row r="8" spans="1:176">
@@ -4490,34 +4521,34 @@
         <v>-42.24922491380607</v>
       </c>
       <c r="DF8">
-        <v>-160396.8907078734</v>
+        <v>-172793.5867078734</v>
       </c>
       <c r="DG8">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DH8">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DI8">
-        <v>-48119.06721236203</v>
+        <v>-51838.07601236203</v>
       </c>
       <c r="DJ8">
-        <v>-16039.68907078734</v>
+        <v>-17279.35867078736</v>
       </c>
       <c r="DK8">
-        <v>144357.2016370861</v>
+        <v>155514.2280370861</v>
       </c>
       <c r="DL8">
-        <v>-47309.20852314814</v>
+        <v>-51028.21732314814</v>
       </c>
       <c r="DM8">
-        <v>-47263.53146582958</v>
+        <v>-50982.54026582958</v>
       </c>
       <c r="DN8">
-        <v>-47224.93900441036</v>
+        <v>-50943.94780441035</v>
       </c>
       <c r="DO8">
-        <v>-15112.0742264016</v>
+        <v>-16351.74382640163</v>
       </c>
       <c r="DP8">
         <v>957.1901644736874</v>
@@ -4553,49 +4584,49 @@
         <v>1084.396772787686</v>
       </c>
       <c r="EA8">
-        <v>-47309.20852314814</v>
+        <v>-51028.21732314814</v>
       </c>
       <c r="EB8">
-        <v>-94572.73998897773</v>
+        <v>-102010.7575889777</v>
       </c>
       <c r="EC8">
-        <v>-141797.6789933881</v>
+        <v>-152954.7053933881</v>
       </c>
       <c r="ED8">
-        <v>-156909.7532197897</v>
+        <v>-169306.4492197897</v>
       </c>
       <c r="EE8">
-        <v>-155952.563055316</v>
+        <v>-168349.259055316</v>
       </c>
       <c r="EF8">
-        <v>-154968.8211171398</v>
+        <v>-167365.5171171398</v>
       </c>
       <c r="EG8">
-        <v>-153961.1090232289</v>
+        <v>-166357.8050232289</v>
       </c>
       <c r="EH8">
-        <v>-152931.4985495052</v>
+        <v>-165328.1945495052</v>
       </c>
       <c r="EI8">
-        <v>-151881.7316564388</v>
+        <v>-164278.4276564388</v>
       </c>
       <c r="EJ8">
-        <v>-150813.2441613229</v>
+        <v>-163209.9401613229</v>
       </c>
       <c r="EK8">
-        <v>-149728.8473885352</v>
+        <v>-162125.5433885352</v>
       </c>
       <c r="EL8">
-        <v>-148644.4506157475</v>
+        <v>-161041.1466157476</v>
       </c>
       <c r="EM8">
-        <v>-147560.0538429599</v>
+        <v>-159956.7498429599</v>
       </c>
       <c r="EN8">
-        <v>-146475.6570701722</v>
+        <v>-158872.3530701722</v>
       </c>
       <c r="EO8">
-        <v>-145391.2602973845</v>
+        <v>-157787.9562973845</v>
       </c>
       <c r="EP8">
         <v>0</v>
@@ -4688,7 +4719,7 @@
         <v>1084.396772787686</v>
       </c>
       <c r="FT8">
-        <v>-45451.11388670214</v>
+        <v>-49650.30372026883</v>
       </c>
     </row>
   </sheetData>
@@ -5115,4 +5146,472 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3">
+        <v>1608</v>
+      </c>
+      <c r="C3">
+        <v>1608</v>
+      </c>
+      <c r="D3">
+        <v>1608</v>
+      </c>
+      <c r="E3">
+        <v>1608</v>
+      </c>
+      <c r="F3">
+        <v>1608</v>
+      </c>
+      <c r="G3">
+        <v>1608</v>
+      </c>
+      <c r="H3">
+        <v>1608</v>
+      </c>
+      <c r="I3">
+        <v>1608</v>
+      </c>
+      <c r="J3">
+        <v>1608</v>
+      </c>
+      <c r="K3">
+        <v>1608</v>
+      </c>
+      <c r="L3">
+        <v>1608</v>
+      </c>
+      <c r="M3">
+        <v>1608</v>
+      </c>
+      <c r="N3">
+        <v>1608</v>
+      </c>
+      <c r="O3">
+        <v>1608</v>
+      </c>
+      <c r="P3">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="C4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="D4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="E4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="F4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="G4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="H4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="I4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="J4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="K4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="L4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="M4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="N4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="O4">
+        <v>32.81632653061224</v>
+      </c>
+      <c r="P4">
+        <v>32.81632653061224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5">
+        <v>88.30886015065067</v>
+      </c>
+      <c r="C5">
+        <v>93.8353731505637</v>
+      </c>
+      <c r="D5">
+        <v>97.89714607092765</v>
+      </c>
+      <c r="E5">
+        <v>101.1680835117484</v>
+      </c>
+      <c r="F5">
+        <v>103.9252635949557</v>
+      </c>
+      <c r="G5">
+        <v>106.3227143668892</v>
+      </c>
+      <c r="H5">
+        <v>108.4373762139851</v>
+      </c>
+      <c r="I5">
+        <v>110.3355575326812</v>
+      </c>
+      <c r="J5">
+        <v>112.0587771467003</v>
+      </c>
+      <c r="K5">
+        <v>113.6415221869177</v>
+      </c>
+      <c r="L5">
+        <v>114.7840268451239</v>
+      </c>
+      <c r="M5">
+        <v>115.3462306069298</v>
+      </c>
+      <c r="N5">
+        <v>115.844019638902</v>
+      </c>
+      <c r="O5">
+        <v>116.3074813602413</v>
+      </c>
+      <c r="P5">
+        <v>116.519065114395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6">
+        <v>55.49253362003843</v>
+      </c>
+      <c r="C6">
+        <v>61.01904661995145</v>
+      </c>
+      <c r="D6">
+        <v>65.0808195403154</v>
+      </c>
+      <c r="E6">
+        <v>68.35175698113621</v>
+      </c>
+      <c r="F6">
+        <v>71.10893706434345</v>
+      </c>
+      <c r="G6">
+        <v>73.50638783627694</v>
+      </c>
+      <c r="H6">
+        <v>75.62104968337287</v>
+      </c>
+      <c r="I6">
+        <v>77.51923100206899</v>
+      </c>
+      <c r="J6">
+        <v>79.24245061608802</v>
+      </c>
+      <c r="K6">
+        <v>80.82519565630548</v>
+      </c>
+      <c r="L6">
+        <v>81.96770031451162</v>
+      </c>
+      <c r="M6">
+        <v>82.52990407631758</v>
+      </c>
+      <c r="N6">
+        <v>83.0276931082898</v>
+      </c>
+      <c r="O6">
+        <v>83.49115482962902</v>
+      </c>
+      <c r="P6">
+        <v>83.70273858378276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7">
+        <v>0.03451028210201395</v>
+      </c>
+      <c r="C7">
+        <v>0.03794716829598971</v>
+      </c>
+      <c r="D7">
+        <v>0.04047314648029565</v>
+      </c>
+      <c r="E7">
+        <v>0.04250731155543296</v>
+      </c>
+      <c r="F7">
+        <v>0.04422197578628324</v>
+      </c>
+      <c r="G7">
+        <v>0.0457129277588787</v>
+      </c>
+      <c r="H7">
+        <v>0.04702801597224681</v>
+      </c>
+      <c r="I7">
+        <v>0.04820847699133644</v>
+      </c>
+      <c r="J7">
+        <v>0.04928013098015424</v>
+      </c>
+      <c r="K7">
+        <v>0.05026442515939396</v>
+      </c>
+      <c r="L7">
+        <v>0.05097493800653707</v>
+      </c>
+      <c r="M7">
+        <v>0.05132456721164028</v>
+      </c>
+      <c r="N7">
+        <v>0.05163413750515534</v>
+      </c>
+      <c r="O7">
+        <v>0.05192235996867477</v>
+      </c>
+      <c r="P7">
+        <v>0.05205394190533754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8">
+        <v>97655.15049561902</v>
+      </c>
+      <c r="C8">
+        <v>107380.6473060155</v>
+      </c>
+      <c r="D8">
+        <v>114528.5106299914</v>
+      </c>
+      <c r="E8">
+        <v>120284.6703727097</v>
+      </c>
+      <c r="F8">
+        <v>125136.7255665259</v>
+      </c>
+      <c r="G8">
+        <v>129355.7330737712</v>
+      </c>
+      <c r="H8">
+        <v>133077.0917404969</v>
+      </c>
+      <c r="I8">
+        <v>136417.4903536592</v>
+      </c>
+      <c r="J8">
+        <v>139449.9932827248</v>
+      </c>
+      <c r="K8">
+        <v>142235.2906014043</v>
+      </c>
+      <c r="L8">
+        <v>144245.8577364896</v>
+      </c>
+      <c r="M8">
+        <v>145235.2177347965</v>
+      </c>
+      <c r="N8">
+        <v>146111.221399815</v>
+      </c>
+      <c r="O8">
+        <v>146926.816241028</v>
+      </c>
+      <c r="P8">
+        <v>147299.1590051156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9">
+        <v>-0.02</v>
+      </c>
+      <c r="C9">
+        <v>-0.02</v>
+      </c>
+      <c r="D9">
+        <v>-0.02</v>
+      </c>
+      <c r="E9">
+        <v>-0.02</v>
+      </c>
+      <c r="F9">
+        <v>-0.02</v>
+      </c>
+      <c r="G9">
+        <v>-0.02</v>
+      </c>
+      <c r="H9">
+        <v>-0.02</v>
+      </c>
+      <c r="I9">
+        <v>-0.02</v>
+      </c>
+      <c r="J9">
+        <v>-0.02</v>
+      </c>
+      <c r="K9">
+        <v>-0.02</v>
+      </c>
+      <c r="L9">
+        <v>-0.02</v>
+      </c>
+      <c r="M9">
+        <v>-0.02</v>
+      </c>
+      <c r="N9">
+        <v>-0.02</v>
+      </c>
+      <c r="O9">
+        <v>-0.02</v>
+      </c>
+      <c r="P9">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10">
+        <v>-0.05205942280040198</v>
+      </c>
+      <c r="C10">
+        <v>-0.05513774988520111</v>
+      </c>
+      <c r="D10">
+        <v>-0.05738748452473071</v>
+      </c>
+      <c r="E10">
+        <v>-0.05919141861336603</v>
+      </c>
+      <c r="F10">
+        <v>-0.06070665922454929</v>
+      </c>
+      <c r="G10">
+        <v>-0.0620202447741322</v>
+      </c>
+      <c r="H10">
+        <v>-0.06317584184351066</v>
+      </c>
+      <c r="I10">
+        <v>-0.06421071661411089</v>
+      </c>
+      <c r="J10">
+        <v>-0.06514822553482019</v>
+      </c>
+      <c r="K10">
+        <v>-0.06600765648505295</v>
+      </c>
+      <c r="L10">
+        <v>-0.06662705542686274</v>
+      </c>
+      <c r="M10">
+        <v>-0.06693154779832435</v>
+      </c>
+      <c r="N10">
+        <v>-0.06720098704937827</v>
+      </c>
+      <c r="O10">
+        <v>-0.06745170604287506</v>
+      </c>
+      <c r="P10">
+        <v>-0.06756612175039409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Profiled and tested Error (should be faster now)
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/output/output_modelo MM - TALCA 28.12_v6 - E1.xlsx
+++ b/Code/Limpio/Excels/output/output_modelo MM - TALCA 28.12_v6 - E1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="238">
   <si>
     <t>LOCALIDAD</t>
   </si>
@@ -551,6 +551,21 @@
     <t>VAN</t>
   </si>
   <si>
+    <t>Usado en E1</t>
+  </si>
+  <si>
+    <t>Usado en E2</t>
+  </si>
+  <si>
+    <t>Usado en E3</t>
+  </si>
+  <si>
+    <t>Usado en E4</t>
+  </si>
+  <si>
+    <t>Usado en E5</t>
+  </si>
+  <si>
     <t>CAUQUENES</t>
   </si>
   <si>
@@ -662,6 +677,15 @@
     <t>V_sub f</t>
   </si>
   <si>
+    <t>V_sub actual</t>
+  </si>
+  <si>
+    <t>Error Actual</t>
+  </si>
+  <si>
+    <t>Decaímiento anual</t>
+  </si>
+  <si>
     <t>Año</t>
   </si>
   <si>
@@ -690,6 +714,15 @@
   </si>
   <si>
     <t>Sin Proyecto - Error ponderado final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>Número de medidores</t>
   </si>
   <si>
     <t>Escenario: medidores con CAPEX ≈ 65% del CAPEX de E1</t>
@@ -1059,13 +1092,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:FT8"/>
+  <dimension ref="A1:FY8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:176">
+    <row r="1" spans="1:181">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1594,19 +1627,34 @@
       <c r="FT1" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:176">
+      <c r="FU1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="FV1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="FW1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="FX1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="FY1" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:181">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>4145544</v>
@@ -1615,10 +1663,10 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1627,19 +1675,19 @@
         <v>2.49041095890411</v>
       </c>
       <c r="K2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AB2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AC2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AU2">
         <v>1</v>
       </c>
       <c r="AV2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="AW2">
         <v>1280.794258147224</v>
@@ -1935,19 +1983,34 @@
       <c r="FT2">
         <v>-63621.97490606039</v>
       </c>
-    </row>
-    <row r="3" spans="1:176">
+      <c r="FU2">
+        <v>0</v>
+      </c>
+      <c r="FV2">
+        <v>0</v>
+      </c>
+      <c r="FW2">
+        <v>0</v>
+      </c>
+      <c r="FX2">
+        <v>0</v>
+      </c>
+      <c r="FY2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:181">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E3">
         <v>1282540</v>
@@ -1956,10 +2019,10 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1968,19 +2031,19 @@
         <v>2.753424657534246</v>
       </c>
       <c r="K3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AB3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AC3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AU3">
         <v>1</v>
       </c>
       <c r="AV3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="AW3">
         <v>1280.794258147224</v>
@@ -2276,19 +2339,34 @@
       <c r="FT3">
         <v>-63621.97490606039</v>
       </c>
-    </row>
-    <row r="4" spans="1:176">
+      <c r="FU3">
+        <v>0</v>
+      </c>
+      <c r="FV3">
+        <v>0</v>
+      </c>
+      <c r="FW3">
+        <v>0</v>
+      </c>
+      <c r="FX3">
+        <v>0</v>
+      </c>
+      <c r="FY3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:181">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B4">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E4">
         <v>1033270</v>
@@ -2297,10 +2375,10 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2309,19 +2387,19 @@
         <v>14.14246575342466</v>
       </c>
       <c r="K4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="AB4" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AC4" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="AU4">
         <v>1</v>
       </c>
       <c r="AV4" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="AW4">
         <v>1280.794258147224</v>
@@ -2617,19 +2695,34 @@
       <c r="FT4">
         <v>-63621.97490606039</v>
       </c>
-    </row>
-    <row r="5" spans="1:176">
+      <c r="FU4">
+        <v>0</v>
+      </c>
+      <c r="FV4">
+        <v>0</v>
+      </c>
+      <c r="FW4">
+        <v>0</v>
+      </c>
+      <c r="FX4">
+        <v>0</v>
+      </c>
+      <c r="FY4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:181">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E5">
         <v>60298899</v>
@@ -2638,10 +2731,10 @@
         <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -2650,7 +2743,7 @@
         <v>1.506849315068493</v>
       </c>
       <c r="K5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="L5">
         <v>-0.04235031726138173</v>
@@ -2701,10 +2794,10 @@
         <v>-0.06709134486990943</v>
       </c>
       <c r="AB5" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AC5" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AD5">
         <v>-0.02</v>
@@ -2761,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="AV5" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="AW5">
         <v>1759.789004486103</v>
@@ -3147,19 +3240,34 @@
       <c r="FT5">
         <v>69440.67433944368</v>
       </c>
-    </row>
-    <row r="6" spans="1:176">
+      <c r="FU5">
+        <v>1</v>
+      </c>
+      <c r="FV5">
+        <v>0</v>
+      </c>
+      <c r="FW5">
+        <v>0</v>
+      </c>
+      <c r="FX5">
+        <v>0</v>
+      </c>
+      <c r="FY5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:181">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E6">
         <v>1245685</v>
@@ -3168,10 +3276,10 @@
         <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H6" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3180,7 +3288,7 @@
         <v>5.534246575342466</v>
       </c>
       <c r="K6" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="L6">
         <v>-0.05783730274303422</v>
@@ -3231,10 +3339,10 @@
         <v>-0.06956789990885255</v>
       </c>
       <c r="AB6" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AC6" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="AD6">
         <v>-0.02</v>
@@ -3291,7 +3399,7 @@
         <v>1</v>
       </c>
       <c r="AV6" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="AW6">
         <v>1759.789004486103</v>
@@ -3677,19 +3785,34 @@
       <c r="FT6">
         <v>368905.2651620624</v>
       </c>
-    </row>
-    <row r="7" spans="1:176">
+      <c r="FU6">
+        <v>1</v>
+      </c>
+      <c r="FV6">
+        <v>1</v>
+      </c>
+      <c r="FW6">
+        <v>1</v>
+      </c>
+      <c r="FX6">
+        <v>1</v>
+      </c>
+      <c r="FY6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:181">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B7">
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E7">
         <v>1244838</v>
@@ -3698,10 +3821,10 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H7" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -3710,7 +3833,7 @@
         <v>4.906849315068493</v>
       </c>
       <c r="K7" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="L7">
         <v>-0.05642172495772248</v>
@@ -3761,10 +3884,10 @@
         <v>-0.06956789990885255</v>
       </c>
       <c r="AB7" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AC7" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="AD7">
         <v>-0.02</v>
@@ -3821,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="AV7" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="AW7">
         <v>1759.789004486103</v>
@@ -4207,19 +4330,34 @@
       <c r="FT7">
         <v>151186.8788804009</v>
       </c>
-    </row>
-    <row r="8" spans="1:176">
+      <c r="FU7">
+        <v>1</v>
+      </c>
+      <c r="FV7">
+        <v>1</v>
+      </c>
+      <c r="FW7">
+        <v>0</v>
+      </c>
+      <c r="FX7">
+        <v>1</v>
+      </c>
+      <c r="FY7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:181">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E8">
         <v>60209613</v>
@@ -4228,10 +4366,10 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="H8" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -4240,7 +4378,7 @@
         <v>5.079452054794521</v>
       </c>
       <c r="K8" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="L8">
         <v>-0.05682844909792741</v>
@@ -4291,10 +4429,10 @@
         <v>-0.06956789990885255</v>
       </c>
       <c r="AB8" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AC8" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="AD8">
         <v>-0.02</v>
@@ -4351,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="AV8" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="AW8">
         <v>1759.789004486103</v>
@@ -4736,6 +4874,21 @@
       </c>
       <c r="FT8">
         <v>-49650.30372026883</v>
+      </c>
+      <c r="FU8">
+        <v>0</v>
+      </c>
+      <c r="FV8">
+        <v>0</v>
+      </c>
+      <c r="FW8">
+        <v>0</v>
+      </c>
+      <c r="FX8">
+        <v>0</v>
+      </c>
+      <c r="FY8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4759,42 +4912,42 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -4829,7 +4982,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -4864,10 +5017,10 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -4902,7 +5055,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4942,13 +5095,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4971,48 +5124,57 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -5029,25 +5191,31 @@
       <c r="K2">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -5064,25 +5232,31 @@
       <c r="K3">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5111,25 +5285,34 @@
       <c r="O4">
         <v>6.085133303522576</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>7.419324184763042</v>
+      </c>
+      <c r="Q4">
+        <v>0.0785784504265742</v>
+      </c>
+      <c r="R4">
+        <v>-2.560753770297293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -5157,6 +5340,15 @@
       </c>
       <c r="O5">
         <v>3.241064640894712</v>
+      </c>
+      <c r="P5">
+        <v>7.419324184763042</v>
+      </c>
+      <c r="Q5">
+        <v>0.1338761216219036</v>
+      </c>
+      <c r="R5">
+        <v>-2.558698845263451</v>
       </c>
     </row>
   </sheetData>
@@ -5166,7 +5358,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5174,7 +5366,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -5224,12 +5416,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>1608</v>
@@ -5279,7 +5471,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>32.81632653061224</v>
@@ -5329,7 +5521,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>88.30886015065067</v>
@@ -5379,7 +5571,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>55.49253362003843</v>
@@ -5429,7 +5621,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>0.03451028210201395</v>
@@ -5479,7 +5671,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>97655.15049561902</v>
@@ -5529,7 +5721,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>-0.02</v>
@@ -5579,7 +5771,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B10">
         <v>-0.05205942280040198</v>
@@ -5625,6 +5817,27 @@
       </c>
       <c r="P10">
         <v>-0.06756612175039409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>1166756.659902354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5634,7 +5847,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5642,7 +5855,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -5692,12 +5905,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>1032</v>
@@ -5747,7 +5960,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>21.06122448979592</v>
@@ -5797,7 +6010,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>62.83630668747166</v>
@@ -5847,7 +6060,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>41.77508219767574</v>
@@ -5897,7 +6110,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>0.04047973081170129</v>
@@ -5947,7 +6160,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>73515.3303129729</v>
@@ -5997,7 +6210,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>-0.02</v>
@@ -6047,7 +6260,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B10">
         <v>-0.05739333478772612</v>
@@ -6093,6 +6306,27 @@
       </c>
       <c r="P10">
         <v>-0.06873112831137719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>345587.1734157469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6102,7 +6336,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6110,7 +6344,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -6160,12 +6394,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>708</v>
@@ -6215,7 +6449,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>14.44897959183674</v>
@@ -6265,7 +6499,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>43.46256804826548</v>
@@ -6315,7 +6549,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>29.01358845642875</v>
@@ -6365,7 +6599,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>0.04097964471246998</v>
@@ -6415,7 +6649,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>51057.79394630823</v>
@@ -6465,7 +6699,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>-0.02</v>
@@ -6515,7 +6749,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B10">
         <v>-0.05783730274303422</v>
@@ -6561,6 +6795,27 @@
       </c>
       <c r="P10">
         <v>-0.06876128892783764</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>172793.5867078734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6570,7 +6825,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6578,7 +6833,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -6628,12 +6883,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>1032</v>
@@ -6683,7 +6938,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>21.06122448979592</v>
@@ -6733,7 +6988,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>62.83630668747166</v>
@@ -6783,7 +7038,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>41.77508219767574</v>
@@ -6833,7 +7088,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>0.04047973081170129</v>
@@ -6883,7 +7138,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>73515.3303129729</v>
@@ -6933,7 +7188,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>-0.02</v>
@@ -6983,7 +7238,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B10">
         <v>-0.05739333478772612</v>
@@ -7029,6 +7284,27 @@
       </c>
       <c r="P10">
         <v>-0.06873112831137719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>345587.1734157469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7038,7 +7314,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7046,7 +7322,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -7096,12 +7372,12 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <v>1968</v>
@@ -7151,7 +7427,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B4">
         <v>33.06122448979592</v>
@@ -7201,7 +7477,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B5">
         <v>89.0318902171565</v>
@@ -7251,7 +7527,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B6">
         <v>55.97066572736058</v>
@@ -7301,7 +7577,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B7">
         <v>0.02844037892650436</v>
@@ -7351,7 +7627,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B8">
         <v>98496.56212077632</v>
@@ -7401,7 +7677,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B9">
         <v>-0.01652184555134011</v>
@@ -7451,7 +7727,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B10">
         <v>-0.04328172579169766</v>
@@ -7497,6 +7773,27 @@
       </c>
       <c r="P10">
         <v>-0.05629804559963512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12">
+        <v>1519338.377610228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>